<commit_message>
added 'path' field to table'
</commit_message>
<xml_diff>
--- a/Parts/RealzingUserCommands.xlsx
+++ b/Parts/RealzingUserCommands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karlm\Desktop\activegits\design\Parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C8F674-7358-4EF2-9B9E-908C995922A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D873AE6-68E0-4BA6-8DA2-9A3453F59137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20040" yWindow="210" windowWidth="17265" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2925" yWindow="1440" windowWidth="18150" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="219">
   <si>
     <t>Controller Method</t>
   </si>
@@ -625,12 +625,105 @@
   <si>
     <t>tbd</t>
   </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>https://commentanywhere.net/….</t>
+  </si>
+  <si>
+    <t>/assignDomainMod</t>
+  </si>
+  <si>
+    <t>/assignGlobalMod</t>
+  </si>
+  <si>
+    <t>/ban</t>
+  </si>
+  <si>
+    <t>/changeEmail</t>
+  </si>
+  <si>
+    <t>/changeFeedback</t>
+  </si>
+  <si>
+    <t>/changeProfile</t>
+  </si>
+  <si>
+    <t>/newComment</t>
+  </si>
+  <si>
+    <t>/voteComment</t>
+  </si>
+  <si>
+    <t>/newFeedback</t>
+  </si>
+  <si>
+    <t>/comments</t>
+  </si>
+  <si>
+    <t>/user</t>
+  </si>
+  <si>
+    <t>/login</t>
+  </si>
+  <si>
+    <t>/logout</t>
+  </si>
+  <si>
+    <t>/moderate</t>
+  </si>
+  <si>
+    <t>/pwResetCode</t>
+  </si>
+  <si>
+    <t>/pwResetReq</t>
+  </si>
+  <si>
+    <t>/newReport</t>
+  </si>
+  <si>
+    <t>/register</t>
+  </si>
+  <si>
+    <t>/reqValidation</t>
+  </si>
+  <si>
+    <t>/newPassword</t>
+  </si>
+  <si>
+    <t>/validate</t>
+  </si>
+  <si>
+    <t>/viewBans</t>
+  </si>
+  <si>
+    <t>/viewCommentReports</t>
+  </si>
+  <si>
+    <t>/viewFeedback</t>
+  </si>
+  <si>
+    <t>/viewLogs</t>
+  </si>
+  <si>
+    <t>/viewModRecords</t>
+  </si>
+  <si>
+    <t>/viewMods</t>
+  </si>
+  <si>
+    <t>/viewDomainReport</t>
+  </si>
+  <si>
+    <t>/viewUsersReport</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -667,6 +760,14 @@
       <color theme="0"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -784,30 +885,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -847,11 +931,33 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="25">
     <dxf>
       <font>
         <b val="0"/>
@@ -870,11 +976,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -888,192 +989,12 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color auto="1"/>
         <name val="Times New Roman"/>
         <family val="1"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1131,12 +1052,18 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color auto="1"/>
+        <color theme="1"/>
         <name val="Times New Roman"/>
         <family val="1"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1169,7 +1096,103 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
         <color auto="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <name val="Times New Roman"/>
         <family val="1"/>
         <scheme val="none"/>
@@ -1223,7 +1246,53 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
         <color auto="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <name val="Times New Roman"/>
         <family val="1"/>
         <scheme val="none"/>
@@ -1261,7 +1330,45 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
         <color auto="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <name val="Times New Roman"/>
         <family val="1"/>
         <scheme val="none"/>
@@ -1335,6 +1442,44 @@
         </top>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1349,18 +1494,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{036517EA-1DC9-4063-84D8-4B45FA209DB8}" name="Table6" displayName="Table6" ref="A4:J32" headerRowCount="0" totalsRowShown="0" headerRowDxfId="20" dataDxfId="21" tableBorderDxfId="22">
-  <tableColumns count="10">
-    <tableColumn id="2" xr3:uid="{92327AEB-30D5-401C-9F6F-8449BB1BF9B9}" name="Column2" headerRowDxfId="1" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{C0F8340D-A57B-43E8-9E15-B80AD5BA22F0}" name="Column3" headerRowDxfId="2" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{171B5E9F-FD4C-4F4B-AC8F-A991FBF52A08}" name="Column4" headerRowDxfId="3" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{DE24E723-9EE4-4541-B2FC-8FBB1966D425}" name="Column5" headerRowDxfId="4" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{89B2560B-4A34-4104-850E-2B31E3564EB5}" name="Column6" headerRowDxfId="5" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{2FA97CFF-6748-4F20-B654-618C7E37AB6A}" name="Column7" headerRowDxfId="6" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{A58A9E2D-B665-45DA-9269-835C80FC0492}" name="Column8" headerRowDxfId="7" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{49E77A9D-419C-4ADF-8961-8F1267C12194}" name="Column9" headerRowDxfId="8" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{58EC5E63-CC1C-4B17-BCD2-4594D982C20F}" name="Column10" headerRowDxfId="9" dataDxfId="12"/>
-    <tableColumn id="11" xr3:uid="{606C6F0E-F3FD-4418-AF41-A68BC93880B8}" name="Column11" headerRowDxfId="10" dataDxfId="11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{036517EA-1DC9-4063-84D8-4B45FA209DB8}" name="Table6" displayName="Table6" ref="A4:K32" headerRowCount="0" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" tableBorderDxfId="22">
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{0944D899-C5BE-4721-8D7B-B1130A8610EF}" name="Column1" headerRowDxfId="2" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{92327AEB-30D5-401C-9F6F-8449BB1BF9B9}" name="Column2" headerRowDxfId="21" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{C0F8340D-A57B-43E8-9E15-B80AD5BA22F0}" name="Column3" headerRowDxfId="20" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{171B5E9F-FD4C-4F4B-AC8F-A991FBF52A08}" name="Column4" headerRowDxfId="18" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{DE24E723-9EE4-4541-B2FC-8FBB1966D425}" name="Column5" headerRowDxfId="16" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{89B2560B-4A34-4104-850E-2B31E3564EB5}" name="Column6" headerRowDxfId="14" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{2FA97CFF-6748-4F20-B654-618C7E37AB6A}" name="Column7" headerRowDxfId="12" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{A58A9E2D-B665-45DA-9269-835C80FC0492}" name="Column8" headerRowDxfId="10" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{49E77A9D-419C-4ADF-8961-8F1267C12194}" name="Column9" headerRowDxfId="8" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{58EC5E63-CC1C-4B17-BCD2-4594D982C20F}" name="Column10" headerRowDxfId="6" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{606C6F0E-F3FD-4418-AF41-A68BC93880B8}" name="Column11" headerRowDxfId="4" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1632,852 +1778,949 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="51.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="29.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="29.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="24.85546875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="19" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="36.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="51.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="29.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="28.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="29.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="5" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="7"/>
-    </row>
-    <row r="2" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="17"/>
+    </row>
+    <row r="2" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="C2" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="D2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="E2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="G2" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="H2" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="I2" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="J2" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="K2" s="13" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="C3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="7"/>
+      <c r="F3" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="G3" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="17"/>
-    </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="H3" s="9"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="11"/>
+    </row>
+    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="G4" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="H4" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="5"/>
+      <c r="J4" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="J4" s="11"/>
-    </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="C5" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D5" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="G5" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="H5" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-    </row>
-    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="E6" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="F6" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="G6" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="H6" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="C7" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="D7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="G7" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="H7" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="G8" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="H8" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="C9" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="D9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="2"/>
+      <c r="F9" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="G9" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="H9" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-    </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="C10" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="D10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="E10" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="F10" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="G10" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="H10" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-    </row>
-    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="C11" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="D11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="E11" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="F11" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="G11" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="H11" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="C12" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="D12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="2"/>
+      <c r="F12" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="G12" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="H12" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-    </row>
-    <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="C13" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="D13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="E13" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="F13" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="G13" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="H13" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11" t="s">
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="C14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="D14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="2"/>
+      <c r="F14" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="G14" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="H14" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="I14" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11" t="s">
+      <c r="J14" s="5"/>
+      <c r="K14" s="5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="C15" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="D15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="E15" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="F15" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="G15" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="H15" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="I15" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11" t="s">
+      <c r="J15" s="5"/>
+      <c r="K15" s="5" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+    <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="C16" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="D16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="E16" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="2"/>
+      <c r="G16" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="H16" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="I16" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-    </row>
-    <row r="17" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="C17" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="D17" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="E17" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="F17" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="G17" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="H17" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11" t="s">
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="C18" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="D18" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="2"/>
+      <c r="F18" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="G18" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="H18" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="C19" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="D19" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="E19" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="F19" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="G19" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="H19" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-    </row>
-    <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+    </row>
+    <row r="20" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="C20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="D20" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="2"/>
+      <c r="F20" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="G20" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="H20" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-    </row>
-    <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="C21" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="2"/>
+      <c r="E21" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="F21" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="G21" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="H21" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="I21" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11" t="s">
+      <c r="J21" s="5"/>
+      <c r="K21" s="5" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="C22" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="D22" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="2"/>
+      <c r="F22" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="G22" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="H22" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="C23" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="D23" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="2"/>
+      <c r="F23" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F23" s="9" t="s">
+      <c r="G23" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="H23" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="C24" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="D24" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="2"/>
+      <c r="F24" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="G24" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="H24" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-    </row>
-    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+    </row>
+    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="C25" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="D25" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="2"/>
+      <c r="F25" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="G25" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="G25" s="10" t="s">
+      <c r="H25" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11" t="s">
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="C26" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="D26" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="2"/>
+      <c r="F26" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F26" s="9" t="s">
+      <c r="G26" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="G26" s="10" t="s">
+      <c r="H26" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11" t="s">
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="C27" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="D27" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="2"/>
+      <c r="F27" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F27" s="9" t="s">
+      <c r="G27" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="G27" s="10" t="s">
+      <c r="H27" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11" t="s">
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="C28" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="D28" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="2"/>
+      <c r="F28" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F28" s="9" t="s">
+      <c r="G28" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G28" s="10" t="s">
+      <c r="H28" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11" t="s">
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="C29" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="D29" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="2"/>
+      <c r="F29" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="F29" s="9" t="s">
+      <c r="G29" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="G29" s="10" t="s">
+      <c r="H29" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11" t="s">
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+    <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="C30" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="D30" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="2"/>
+      <c r="F30" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F30" s="9" t="s">
+      <c r="G30" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="G30" s="10" t="s">
+      <c r="H30" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11" t="s">
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="C31" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="D31" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="2"/>
+      <c r="F31" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F31" s="9" t="s">
+      <c r="G31" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="G31" s="10" t="s">
+      <c r="H31" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11" t="s">
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="C32" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="D32" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8" t="s">
+      <c r="E32" s="2"/>
+      <c r="F32" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F32" s="9" t="s">
+      <c r="G32" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="G32" s="10" t="s">
+      <c r="H32" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11" t="s">
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5" t="s">
         <v>160</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="B1:G1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{918B44D3-436F-4138-9C40-E4650A7F0556}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="42" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="42" orientation="landscape" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>